<commit_message>
actualizacion de ultimos archivos
carga de powe bi y memv
</commit_message>
<xml_diff>
--- a/PROYECTO_FINAL/Datos/CLAVES_NOMBRES.xlsx
+++ b/PROYECTO_FINAL/Datos/CLAVES_NOMBRES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanj\Workspace\business_Intelligence\PROYECTO_FINAL\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF2607A-7A01-483F-96C3-D74982692597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE6BF66-A335-46D5-A7EF-BFAA4A1A6222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="210" yWindow="825" windowWidth="21600" windowHeight="11505" xr2:uid="{7179F0DD-434A-4961-8AF4-FEC02D6131C3}"/>
+    <workbookView xWindow="5670" yWindow="2460" windowWidth="21600" windowHeight="11505" xr2:uid="{7179F0DD-434A-4961-8AF4-FEC02D6131C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1046,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02880842-5284-4274-9BDE-6551DF7F08D8}">
   <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>